<commit_message>
export datasheets as PDFS (fouling community)
</commit_message>
<xml_diff>
--- a/fouling/original_datasheets/Fouling Community Data Sheets.xlsx
+++ b/fouling/original_datasheets/Fouling Community Data Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dean/Documents/TMON WG/Fouling Community Protocol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\fouling\original_datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9511B016-E398-9E46-9CD6-1B2A93435364}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660F3302-9890-4208-8F84-B4DF5536A94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="2100" windowWidth="29540" windowHeight="19500" xr2:uid="{866B0E7E-65EB-2142-8794-205B7BF0606A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{866B0E7E-65EB-2142-8794-205B7BF0606A}"/>
   </bookViews>
   <sheets>
     <sheet name="Species List" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
-  <si>
-    <t>Species List</t>
-  </si>
   <si>
     <t>Genus</t>
   </si>
@@ -65,9 +62,6 @@
     <t>Weight of Panel (g)</t>
   </si>
   <si>
-    <t>Species Richenss:</t>
-  </si>
-  <si>
     <t>Community Biomass (g)</t>
   </si>
   <si>
@@ -77,10 +71,16 @@
     <t>Habitat:</t>
   </si>
   <si>
-    <t>Percent Cover</t>
+    <t>Species Richness:</t>
   </si>
   <si>
-    <t>Mesofauna Counts</t>
+    <t>Fouling Community Species List</t>
+  </si>
+  <si>
+    <t>Fouling Community Percent Cover</t>
+  </si>
+  <si>
+    <t>Fouling Community Mesofauna Counts</t>
   </si>
 </sst>
 </file>
@@ -332,18 +332,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -361,10 +349,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,64 +679,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D39263E-1ADE-7043-9375-0A9D035AEE13}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="9" width="12.33203125" customWidth="1"/>
+    <col min="4" max="9" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
@@ -745,7 +749,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -756,7 +760,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -767,7 +771,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -778,7 +782,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -789,7 +793,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -800,7 +804,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -811,7 +815,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -822,7 +826,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -833,7 +837,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -844,7 +848,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -855,7 +859,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -866,7 +870,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -877,7 +881,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -888,7 +892,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -899,7 +903,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -910,7 +914,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -921,7 +925,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -932,7 +936,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -943,7 +947,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -954,7 +958,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -965,7 +969,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -976,7 +980,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
@@ -987,11 +991,11 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1000,7 +1004,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1011,12 +1015,12 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
-      <c r="B29" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="13"/>
+      <c r="B29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="23"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1024,12 +1028,12 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="12"/>
+      <c r="B30" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="22"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1037,11 +1041,11 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="12"/>
+    <row r="31" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="22"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1049,109 +1053,109 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1162,344 +1166,354 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="81" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;Lhttps://doi.org/10.25573/serc.14510649.v1</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4586FBBA-1F0E-424A-9665-7F8A0C9A9670}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I26"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="24" t="s">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="92" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;Lhttps://doi.org/10.25573/serc.14510649.v1</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1507,329 +1521,333 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16C75B-F2D3-E84B-AB00-2509388F6DA7}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="24" t="s">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="C1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;Lhttps://doi.org/10.25573/serc.14510649.v1</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>